<commit_message>
add reduced HuangZhou element
</commit_message>
<xml_diff>
--- a/fem3d/errorPoisson.xlsx
+++ b/fem3d/errorPoisson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangxuehai/work/paper/Program/femcode/fem3d/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B80A1315-773D-2A4E-B94C-CDA352BCDA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4760B482-6352-A546-9E73-0D3AF7607E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="500" windowWidth="28800" windowHeight="16040"/>
+    <workbookView xWindow="500" yWindow="1660" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="error" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t>k=1</t>
   </si>
@@ -75,14 +78,18 @@
     <t>k=6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>rel. res.=1e-12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="184" formatCode="#\ ???/???"/>
-    <numFmt numFmtId="185" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="176" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="177" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -93,11 +100,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -127,14 +136,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="184" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -506,11 +513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40:D40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -565,14 +572,12 @@
       <c r="D3" s="2">
         <v>1.5452049999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>27</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
@@ -588,21 +593,21 @@
       <c r="D4" s="2">
         <v>0.91585810000000001</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>125</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4">
         <f t="shared" ref="G4:I8" si="0">LOG(B3/B4,2)</f>
         <v>1.432208231522716</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>0.74424833178144556</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>0.75460225659615832</v>
       </c>
@@ -621,21 +626,21 @@
       <c r="D5" s="2">
         <v>0.47983209999999998</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>729</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>1.8287992996246989</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>0.92791748430902854</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5">
         <f t="shared" si="0"/>
         <v>0.93259441442735425</v>
       </c>
@@ -654,21 +659,21 @@
       <c r="D6" s="2">
         <v>0.242838</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>4913</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>1.953285982125502</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>0.98113715671128332</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <f t="shared" si="0"/>
         <v>0.98253547845478373</v>
       </c>
@@ -687,21 +692,21 @@
       <c r="D7" s="2">
         <v>0.1217911</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>35937</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>1.9879726062163898</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>0.99521846781780543</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <f t="shared" si="0"/>
         <v>0.99558548560626747</v>
       </c>
@@ -720,21 +725,21 @@
       <c r="D8" s="2">
         <v>6.094227E-2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>274625</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>1.996967605561218</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>0.9988001940555512</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <f t="shared" si="0"/>
         <v>0.99889356661808293</v>
       </c>
@@ -744,10 +749,6 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
@@ -791,14 +792,12 @@
       <c r="D13" s="2">
         <v>0.5747274</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="4">
         <v>125</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
@@ -814,21 +813,21 @@
       <c r="D14" s="2">
         <v>0.1690731</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="4">
         <v>729</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14">
         <f t="shared" ref="G14:I17" si="1">LOG(B13/B14,2)</f>
         <v>2.9385443537074689</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14">
         <f t="shared" si="1"/>
         <v>1.7619102378892835</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14">
         <f t="shared" si="1"/>
         <v>1.765230689759461</v>
       </c>
@@ -847,21 +846,21 @@
       <c r="D15" s="2">
         <v>4.4987649999999997E-2</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="4">
         <v>4913</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15">
         <f t="shared" si="1"/>
         <v>3.0081639130932487</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15">
         <f t="shared" si="1"/>
         <v>1.909412932114106</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15">
         <f t="shared" si="1"/>
         <v>1.910046228641932</v>
       </c>
@@ -880,21 +879,21 @@
       <c r="D16" s="2">
         <v>1.1474949999999999E-2</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>2</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>35937</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>3.0039276204944496</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16">
         <f t="shared" si="1"/>
         <v>1.9709071781200269</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16">
         <f t="shared" si="1"/>
         <v>1.971041140089167</v>
       </c>
@@ -913,21 +912,21 @@
       <c r="D17" s="2">
         <v>2.8850130000000001E-3</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>3</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>274625</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17">
         <f t="shared" si="1"/>
         <v>3.0005596252136675</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17">
         <f t="shared" si="1"/>
         <v>1.9918058965961889</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17">
         <f t="shared" si="1"/>
         <v>1.9918381425248703</v>
       </c>
@@ -974,14 +973,12 @@
       <c r="D22" s="2">
         <v>0.16222249999999999</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
         <v>2</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>343</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
@@ -997,21 +994,21 @@
       <c r="D23" s="2">
         <v>2.2416910000000002E-2</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
         <v>3</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="4">
         <v>2197</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23">
         <f t="shared" ref="G23:I25" si="2">LOG(B22/B23,2)</f>
         <v>3.9701349585189787</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23">
         <f t="shared" si="2"/>
         <v>2.8536078316383517</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23">
         <f t="shared" si="2"/>
         <v>2.8553146004592169</v>
       </c>
@@ -1030,21 +1027,21 @@
       <c r="D24" s="2">
         <v>2.8115689999999999E-3</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
         <v>3</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <v>15625</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24">
         <f t="shared" si="2"/>
         <v>4.1100813839506429</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24">
         <f t="shared" si="2"/>
         <v>2.9947764325694268</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24">
         <f t="shared" si="2"/>
         <v>2.9951400690803207</v>
       </c>
@@ -1063,21 +1060,21 @@
       <c r="D25" s="2">
         <v>3.4888729999999998E-4</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25">
         <v>4</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="4">
         <v>117649</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25">
         <f t="shared" si="2"/>
         <v>4.0712231755651329</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25">
         <f t="shared" si="2"/>
         <v>3.0104662716549608</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25">
         <f t="shared" si="2"/>
         <v>3.0105424657273834</v>
       </c>
@@ -1124,14 +1121,12 @@
       <c r="D30" s="2">
         <v>3.5848100000000001E-2</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30">
         <v>4</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="4">
         <v>729</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
@@ -1147,21 +1142,21 @@
       <c r="D31" s="2">
         <v>2.4670600000000001E-3</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
         <v>5</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="4">
         <v>4913</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31">
         <f t="shared" ref="G31:I33" si="3">LOG(B30/B31,2)</f>
         <v>4.9029447675810607</v>
       </c>
-      <c r="H31" s="4">
+      <c r="H31">
         <f t="shared" si="3"/>
         <v>3.8600098146826425</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31">
         <f t="shared" si="3"/>
         <v>3.8610319479114401</v>
       </c>
@@ -1180,21 +1175,21 @@
       <c r="D32" s="2">
         <v>1.586061E-4</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
         <v>6</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="4">
         <v>35937</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32">
         <f t="shared" si="3"/>
         <v>4.949855313244087</v>
       </c>
-      <c r="H32" s="4">
+      <c r="H32">
         <f t="shared" si="3"/>
         <v>3.9590368700394518</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32">
         <f t="shared" si="3"/>
         <v>3.9592726396935549</v>
       </c>
@@ -1213,27 +1208,27 @@
       <c r="D33" s="2">
         <v>9.988248E-6</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
         <v>6</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="4">
         <v>274625</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33">
         <f t="shared" si="3"/>
         <v>4.9814067240979849</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33">
         <f t="shared" si="3"/>
         <v>3.9890128347761129</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33">
         <f t="shared" si="3"/>
         <v>3.9890728053757547</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
@@ -1274,14 +1269,12 @@
       <c r="D37" s="2">
         <v>6.9217810000000001E-3</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37">
         <v>8</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="4">
         <v>1331</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
@@ -1297,21 +1290,21 @@
       <c r="D38" s="2">
         <v>2.3495739999999999E-4</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38">
         <v>9</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="4">
         <v>9261</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38">
         <f t="shared" ref="G38:I40" si="4">LOG(B37/B38,2)</f>
         <v>5.9022189335254156</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38">
         <f t="shared" si="4"/>
         <v>4.8799733140031796</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38">
         <f t="shared" si="4"/>
         <v>4.8806721850779429</v>
       </c>
@@ -1330,21 +1323,21 @@
       <c r="D39" s="2">
         <v>7.3970179999999997E-6</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39">
         <v>11</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="4">
         <v>68921</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39">
         <f t="shared" si="4"/>
         <v>6.0151896453012181</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39">
         <f t="shared" si="4"/>
         <v>4.9891414997129377</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39">
         <f t="shared" si="4"/>
         <v>4.9893116095493042</v>
       </c>
@@ -1363,31 +1356,31 @@
       <c r="D40" s="2">
         <v>2.303239E-7</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40">
         <v>16</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="4">
         <v>531441</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40">
         <f t="shared" si="4"/>
         <v>6.0132419114465963</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40">
         <f t="shared" si="4"/>
         <v>5.005166886043301</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40">
         <f t="shared" si="4"/>
         <v>5.0052077584414674</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C42" t="s">
-        <v>1</v>
+      <c r="C42" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1424,14 +1417,12 @@
       <c r="D44" s="2">
         <v>1.0791419999999999E-3</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44">
         <v>14</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="4">
         <v>2197</v>
       </c>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1">
@@ -1447,21 +1438,21 @@
       <c r="D45" s="2">
         <v>1.8128800000000002E-5</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45">
         <v>16</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="4">
         <v>15625</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45">
         <f t="shared" ref="G45:I47" si="5">LOG(B44/B45,2)</f>
         <v>6.8868094904897381</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45">
         <f t="shared" si="5"/>
         <v>5.8947805280724523</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45">
         <f t="shared" si="5"/>
         <v>5.8954574736867373</v>
       </c>
@@ -1480,21 +1471,21 @@
       <c r="D46" s="2">
         <v>2.8894559999999998E-7</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46">
         <v>17</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="4">
         <v>117649</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46">
         <f t="shared" si="5"/>
         <v>6.9608483742319072</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46">
         <f t="shared" si="5"/>
         <v>5.9711717260090982</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46">
         <f t="shared" si="5"/>
         <v>5.9713417206389892</v>
       </c>
@@ -1504,22 +1495,32 @@
         <f>1/2^4</f>
         <v>6.25E-2</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="4" t="e">
+      <c r="B47" s="2">
+        <v>2.0409990000000001E-11</v>
+      </c>
+      <c r="C47" s="2">
+        <v>4.5310340000000003E-9</v>
+      </c>
+      <c r="D47" s="2">
+        <v>4.53108E-9</v>
+      </c>
+      <c r="E47">
+        <v>31</v>
+      </c>
+      <c r="F47" s="4">
+        <v>912673</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H47" s="4" t="e">
+        <v>6.9889252597875737</v>
+      </c>
+      <c r="H47">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I47" s="4" t="e">
+        <v>5.9947553553533028</v>
+      </c>
+      <c r="I47">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>5.9947991277514667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>